<commit_message>
Some plots being created
</commit_message>
<xml_diff>
--- a/Nike.xlsx
+++ b/Nike.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julioguzman/Repos/ScrapeStocksData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B392C9C-39CC-EF4B-8A8C-673FFF4F2567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E93BCD-9F1D-324A-B6D1-2B10563348A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{C86735B1-B838-5D45-8266-C8E330DD1CE2}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{C86735B1-B838-5D45-8266-C8E330DD1CE2}"/>
   </bookViews>
   <sheets>
-    <sheet name="NKE Balance Annual" sheetId="1" r:id="rId1"/>
-    <sheet name="NKE Income Annual" sheetId="2" r:id="rId2"/>
+    <sheet name="NKE Income Annual" sheetId="2" r:id="rId1"/>
+    <sheet name="NKE Balance Annual" sheetId="1" r:id="rId2"/>
     <sheet name="NKE Cash Annual" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -579,402 +579,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BFF54E-F404-5D48-AFC7-14DBF57A6ADC}">
-  <dimension ref="A1:A76"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>45077</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>44712</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>44347</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>43982</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>37531000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>40321000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>37740000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>31342000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>23527000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>25040000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>24973000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>23287000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>14004000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>15281000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>12767000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>8055000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>22931000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>24201000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <v>22180000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>17461000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
-        <v>14004000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <v>15281000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>12767000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>8055000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>3211000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
-        <v>3197000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
-        <v>3398000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
-        <v>3358000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <v>13449000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
-        <v>14711000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <v>12256000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <v>7558000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <v>15946000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <v>17483000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <v>16617000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <v>12272000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>22937000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
-        <v>24711000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
-        <v>22182000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
-        <v>17712000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
-        <v>13449000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
-        <v>14711000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A54" s="3">
-        <v>12256000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
-        <v>7558000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
-        <v>12144000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
-        <v>12627000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
-        <v>12813000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
-        <v>13015000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
-        <v>1492000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
-        <v>856000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
-        <v>1309000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
-        <v>1532000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A68" s="3">
-        <v>1571000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A69" s="3">
-        <v>1578000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
-        <v>1558000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
-        <v>1532000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A73" s="3">
-        <v>1571000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A74" s="3">
-        <v>1578000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A75" s="3">
-        <v>1558000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F0FF47-AA9B-E046-855F-494ABCF665EC}">
   <dimension ref="A1:A161"/>
   <sheetViews>
@@ -1791,6 +1395,402 @@
       <c r="A161" s="1">
         <v>0</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BFF54E-F404-5D48-AFC7-14DBF57A6ADC}">
+  <dimension ref="A1:A76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>45077</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>43982</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>37531000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>40321000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>37740000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>31342000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>23527000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>25040000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>24973000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>23287000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>14004000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>15281000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>12767000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>8055000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>22931000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>24201000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>22180000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>17461000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>14004000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>15281000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>12767000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>8055000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>3211000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>3197000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>3398000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>3358000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>13449000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>14711000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>12256000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>7558000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>15946000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>17483000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>16617000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>12272000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>22937000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>24711000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>22182000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>17712000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>13449000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>14711000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>12256000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>7558000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>12144000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>12627000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>12813000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>13015000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>1492000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>856000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>1309000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>1532000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>1571000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>1578000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>1558000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
+        <v>1532000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>1571000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>1578000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>1558000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Not showing plots and auto closing them
</commit_message>
<xml_diff>
--- a/Nike.xlsx
+++ b/Nike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julioguzman/Repos/ScrapeStocksData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E93BCD-9F1D-324A-B6D1-2B10563348A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1ACBF-B337-324B-BC57-50F185553044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{C86735B1-B838-5D45-8266-C8E330DD1CE2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>Breakdown</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>Normalized EBITDA</t>
-  </si>
-  <si>
-    <t>Tax Rate for Calcs</t>
   </si>
   <si>
     <t>Operating Cash Flow</t>
@@ -580,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F0FF47-AA9B-E046-855F-494ABCF665EC}">
-  <dimension ref="A1:A161"/>
+  <dimension ref="A1:A156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1371,31 +1368,6 @@
         <v>4234000</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A157" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A158" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A159" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A160" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A161" s="1">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1403,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BFF54E-F404-5D48-AFC7-14DBF57A6ADC}">
-  <dimension ref="A1:A76"/>
+  <dimension ref="A1:A77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1420,377 +1392,382 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>45077</v>
+      <c r="A2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44712</v>
+        <v>45077</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44347</v>
+        <v>44712</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
+        <v>44347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>43982</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>37531000</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>40321000</v>
+        <v>37531000</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>37740000</v>
+        <v>40321000</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
+        <v>37740000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>31342000</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>23527000</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>25040000</v>
+        <v>23527000</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>24973000</v>
+        <v>25040000</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
+        <v>24973000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <v>23287000</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>14004000</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>15281000</v>
+        <v>14004000</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>12767000</v>
+        <v>15281000</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
+        <v>12767000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>8055000</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>22931000</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <v>24201000</v>
+        <v>22931000</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>22180000</v>
+        <v>24201000</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
+        <v>22180000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>17461000</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
-        <v>14004000</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
-        <v>15281000</v>
+        <v>14004000</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
-        <v>12767000</v>
+        <v>15281000</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
+        <v>12767000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
         <v>8055000</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>3211000</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
-        <v>3197000</v>
+        <v>3211000</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
-        <v>3398000</v>
+        <v>3197000</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
+        <v>3398000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>3358000</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <v>13449000</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
-        <v>14711000</v>
+        <v>13449000</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
-        <v>12256000</v>
+        <v>14711000</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
+        <v>12256000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
         <v>7558000</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <v>15946000</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
-        <v>17483000</v>
+        <v>15946000</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
-        <v>16617000</v>
+        <v>17483000</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
+        <v>16617000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
         <v>12272000</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>22937000</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
-        <v>24711000</v>
+        <v>22937000</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
-        <v>22182000</v>
+        <v>24711000</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
+        <v>22182000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
         <v>17712000</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
-        <v>13449000</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
-        <v>14711000</v>
+        <v>13449000</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
-        <v>12256000</v>
+        <v>14711000</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
+        <v>12256000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
         <v>7558000</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
-        <v>12144000</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
-        <v>12627000</v>
+        <v>12144000</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
-        <v>12813000</v>
+        <v>12627000</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
+        <v>12813000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
         <v>13015000</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
-        <v>1492000</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
+        <v>1492000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
         <v>856000</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
         <v>1309000</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
-        <v>1532000</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
-        <v>1571000</v>
+        <v>1532000</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
-        <v>1578000</v>
+        <v>1571000</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
+        <v>1578000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
         <v>1558000</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
-        <v>1532000</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
-        <v>1571000</v>
+        <v>1532000</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
-        <v>1578000</v>
+        <v>1571000</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
+        <v>1578000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
         <v>1558000</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
+    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1802,7 +1779,7 @@
   <dimension ref="A1:A73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:XFD78"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1842,7 +1819,7 @@
     </row>
     <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -1872,7 +1849,7 @@
     </row>
     <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -1902,7 +1879,7 @@
     </row>
     <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -1932,7 +1909,7 @@
     </row>
     <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -1962,7 +1939,7 @@
     </row>
     <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -1992,7 +1969,7 @@
     </row>
     <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -2022,7 +1999,7 @@
     </row>
     <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -2052,7 +2029,7 @@
     </row>
     <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -2082,7 +2059,7 @@
     </row>
     <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -2112,7 +2089,7 @@
     </row>
     <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -2142,7 +2119,7 @@
     </row>
     <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Putting plots into folders
</commit_message>
<xml_diff>
--- a/Nike.xlsx
+++ b/Nike.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julioguzman/Repos/ScrapeStocksData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1ACBF-B337-324B-BC57-50F185553044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F0730C-BECA-D24E-96A8-699274DC3A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="1" xr2:uid="{C86735B1-B838-5D45-8266-C8E330DD1CE2}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{C86735B1-B838-5D45-8266-C8E330DD1CE2}"/>
   </bookViews>
   <sheets>
-    <sheet name="NKE Income Annual" sheetId="2" r:id="rId1"/>
-    <sheet name="NKE Balance Annual" sheetId="1" r:id="rId2"/>
-    <sheet name="NKE Cash Annual" sheetId="3" r:id="rId3"/>
+    <sheet name="NKE Income" sheetId="2" r:id="rId1"/>
+    <sheet name="NKE Balance" sheetId="1" r:id="rId2"/>
+    <sheet name="NKE Cash" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F0FF47-AA9B-E046-855F-494ABCF665EC}">
   <dimension ref="A1:A156"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139:A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1377,7 +1377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BFF54E-F404-5D48-AFC7-14DBF57A6ADC}">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1778,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F730F5C-8E26-154D-9D70-56405CCEC6B1}">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
More data and code slightly adjusted
</commit_message>
<xml_diff>
--- a/Nike.xlsx
+++ b/Nike.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julioguzman/Repos/ScrapeStocksData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F0730C-BECA-D24E-96A8-699274DC3A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6F7087-6C5E-0C46-B115-782247AA68D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{C86735B1-B838-5D45-8266-C8E330DD1CE2}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="8" xr2:uid="{C86735B1-B838-5D45-8266-C8E330DD1CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="NKE Income" sheetId="2" r:id="rId1"/>
     <sheet name="NKE Balance" sheetId="1" r:id="rId2"/>
     <sheet name="NKE Cash" sheetId="3" r:id="rId3"/>
+    <sheet name="ADDYY Income" sheetId="4" r:id="rId4"/>
+    <sheet name="ADDYY Balance" sheetId="5" r:id="rId5"/>
+    <sheet name="ADDYY Cash" sheetId="6" r:id="rId6"/>
+    <sheet name="DECK Income" sheetId="7" r:id="rId7"/>
+    <sheet name="DECK Balance" sheetId="8" r:id="rId8"/>
+    <sheet name="DECK Cash" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="63">
   <si>
     <t>Breakdown</t>
   </si>
@@ -198,12 +204,42 @@
   <si>
     <t>Free Cash Flow</t>
   </si>
+  <si>
+    <t>Total Operating Income as Reported</t>
+  </si>
+  <si>
+    <t>Rent Expense Supplemental</t>
+  </si>
+  <si>
+    <t>Interest Income</t>
+  </si>
+  <si>
+    <t>Interest Expense</t>
+  </si>
+  <si>
+    <t>Total Unusual Items Excluding Goodwill</t>
+  </si>
+  <si>
+    <t>Total Unusual Items</t>
+  </si>
+  <si>
+    <t>Tax Rate for Calcs</t>
+  </si>
+  <si>
+    <t>Tax Effect of Unusual Items</t>
+  </si>
+  <si>
+    <t>Treasury Shares Number</t>
+  </si>
+  <si>
+    <t>Issuance of Capital Stock</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +250,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FF232A31"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -238,11 +280,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F0FF47-AA9B-E046-855F-494ABCF665EC}">
   <dimension ref="A1:A156"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139:A144"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1377,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BFF54E-F404-5D48-AFC7-14DBF57A6ADC}">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1778,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F730F5C-8E26-154D-9D70-56405CCEC6B1}">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2153,4 +2200,4047 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979C1990-46A1-1743-A92D-A50D31BC90A4}">
+  <dimension ref="A1:A230"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.33203125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>44926</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>21611000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>21427000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>22511000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>21234000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>18435000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>10995000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>11244000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>11867000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>10469000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>9213000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>10616000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>10183000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>10644000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>10765000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>9222000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>10061000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>9904000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>9915000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>8776000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>8369000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>555000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>279000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>729000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
+        <v>1989000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>853000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>-146000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>-83000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>-115000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>-96000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>-212000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>278000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>388000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
+        <v>1852000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>578000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>143000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <v>124000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <v>134000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <v>117000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <v>134000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>-75000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <v>612000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
+        <v>2116000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="7">
+        <v>432000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="7">
+        <v>134000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="7">
+        <v>-75000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="7">
+        <v>612000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="7">
+        <v>2116000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="7">
+        <v>432000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="5">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="5">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="5">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="5">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="8">
+        <v>357924.51</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="8">
+        <v>366527.26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="8">
+        <v>388345.97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="8">
+        <v>390311.85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="8">
+        <v>395212.21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="8">
+        <v>357952.55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="8">
+        <v>366536.17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="8">
+        <v>388356.16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="8">
+        <v>390323.46</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="8">
+        <v>395225.07</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="7">
+        <v>544000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="7">
+        <v>268000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="7">
+        <v>669000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="7">
+        <v>1986000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="7">
+        <v>746000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="7">
+        <v>142000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="7">
+        <v>132000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="7">
+        <v>21056000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="7">
+        <v>21148000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="7">
+        <v>21782000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="7">
+        <v>19245000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="7">
+        <v>17582000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="7">
+        <v>134000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="7">
+        <v>-75000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="7">
+        <v>612000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="7">
+        <v>2116000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="7">
+        <v>432000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="7">
+        <v>95200</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="7">
+        <v>-108800</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="7">
+        <v>267300</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="7">
+        <v>1450806</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="7">
+        <v>537184</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="7">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="7">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="7">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="7">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="7">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="7">
+        <v>234000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="7">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="7">
+        <v>137000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="7">
+        <v>111000</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="7">
+        <v>238000</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="7">
+        <v>-146000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="7">
+        <v>-83000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="7">
+        <v>-115000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="7">
+        <v>-96000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="7">
+        <v>-212000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="7">
+        <v>512000</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="7">
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="7">
+        <v>525000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="7">
+        <v>1963000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="7">
+        <v>816000</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="7">
+        <v>1716000</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="7">
+        <v>1437000</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="7">
+        <v>1900000</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="7">
+        <v>3112000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="7">
+        <v>2077000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="7">
+        <v>10995000</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="7">
+        <v>11244000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="7">
+        <v>11867000</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="7">
+        <v>10469000</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="7">
+        <v>9213000</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="7">
+        <v>1204000</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="7">
+        <v>1212000</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" s="7">
+        <v>1375000</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" s="7">
+        <v>1149000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" s="7">
+        <v>1261000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" s="7">
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" s="7">
+        <v>-119000</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" s="7">
+        <v>228000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" s="7">
+        <v>1450000</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" s="7">
+        <v>451000</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" s="7">
+        <v>-12000</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" s="7">
+        <v>-12000</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" s="7">
+        <v>-60000</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" s="7">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" s="7">
+        <v>-108000</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" s="7">
+        <v>-12000</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" s="7">
+        <v>-12000</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" s="7">
+        <v>-60000</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" s="7">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="7">
+        <v>-108000</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="7">
+        <v>1728000</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="7">
+        <v>1449000</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" s="7">
+        <v>1960000</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" s="7">
+        <v>3113000</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" s="7">
+        <v>2185000</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A226" s="3">
+        <v>-1800</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A227" s="3">
+        <v>-1800</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A228" s="3">
+        <v>-20700</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>-194</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A230" s="3">
+        <v>-21816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7EE91A-5317-8449-BBBC-7A266A60C15B}">
+  <dimension ref="A1:A96"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="135.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>44926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>18020000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>20296000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>22137000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>21053000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>13095000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>14945000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>14300000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>14362000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>4925000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>5351000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>7837000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>6691000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>7010000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>7937000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>9985000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>8936000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>4580000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>4991000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>7519000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>6454000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>2584000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>2986000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>2836000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>2722000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>2900000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>3302000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>5938000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>4245000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>1766000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>2475000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>4979000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>3327000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>7559000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>8464000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>10014000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>9622000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>2900000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>3302000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>5938000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>4245000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>5563000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>6459000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>5331000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
+        <v>5890000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>1548000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>2675000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
+        <v>192100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>200416.19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>178549.08</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>178537.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="3">
+        <v>192100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>195066.06</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>1450.92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <v>1462.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <v>5350.13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>4446.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F3CCA1-1632-A94F-9428-120C23DECA7C}">
+  <dimension ref="A1:A76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44926</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>3052000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>2630000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>-479000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>3192000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>1486000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>-519000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>-450000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>495000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>-424000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>-115000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>-2084000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>-1425000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>-2963000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>-2991000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>479000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>1227000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>1431000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>798000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>3828000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>3994000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>-495000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>-504000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>-695000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>-667000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>-432000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>-648000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>994000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>1501000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>-500000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>-679000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>-519000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>-37000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>-29000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>-2530000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>-1032000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>-286000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
+        <v>2557000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>2126000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>-1174000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>2525000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>1054000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A41E26-BFC1-2141-B554-9D3672BCA6FA}">
+  <dimension ref="A1:A210"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>4287763</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>4287763</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>3627286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>3150339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>2545641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>1902275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>1902275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>1801916</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>1542788</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>1171551</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>2385488</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>2385488</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>1825370</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>1607551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>1374090</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>1457974</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>1457974</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>1172619</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>1042844</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>869885</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>927514</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>927514</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>652751</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>564707</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>504205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>49644</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>49644</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>12121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>-182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>-3391</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>978941</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>978941</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>666082</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>564638</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>501514</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>219378</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>219378</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>149260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>112689</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>118939</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>516822</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>451949</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>382575</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
+        <v>516822</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
+        <v>451949</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="3">
+        <v>382575</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>29.36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>16.43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>13.64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>9.73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>29.16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>19.37</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>16.260000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>13.47</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>9.6199999999999992</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A100" s="3">
+        <v>25871</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A102" s="3">
+        <v>26504</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A103" s="3">
+        <v>27508</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A104" s="3">
+        <v>28055</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A105" s="3">
+        <v>28385</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>26048</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>26686</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>27789</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>28406</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>28694</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>927514</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>927514</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>652751</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>564707</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>504205</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>3360249</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>3360249</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>2974535</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>2585632</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>2041436</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>516822</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>451949</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>382575</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>516822</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>451949</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>382575</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>52208</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>52208</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>15563</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>3442</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>6028</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>49644</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>49644</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>12121</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>-182</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>-3391</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
+        <v>981505</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
+        <v>981505</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
+        <v>669524</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
+        <v>566721</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A167" s="3">
+        <v>507542</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A170" s="3">
+        <v>1038671</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A171" s="3">
+        <v>1038671</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A172" s="3">
+        <v>716869</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A173" s="3">
+        <v>609599</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A174" s="3">
+        <v>548072</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
+        <v>1902275</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
+        <v>1902275</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>1801916</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
+        <v>1542788</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A181" s="3">
+        <v>1171551</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A184" s="3">
+        <v>57166</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A185" s="3">
+        <v>57166</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A186" s="3">
+        <v>47345</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A187" s="3">
+        <v>42878</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A188" s="3">
+        <v>40530</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A191" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A192" s="3">
+        <v>759563</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A193" s="3">
+        <v>516822</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A194" s="3">
+        <v>451949</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A195" s="3">
+        <v>382575</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A198" s="3">
+        <v>1038671</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A199" s="3">
+        <v>1038671</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A200" s="3">
+        <v>716869</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A201" s="3">
+        <v>609599</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A202" s="3">
+        <v>548072</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8689B3B-7C01-EA4E-B2B2-9976ADD0346F}">
+  <dimension ref="A1:A84"/>
+  <sheetViews>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>45382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>3135579</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>2556203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>2332250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>2167705</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>1028111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>790470</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>793425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>723480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>2107468</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>1765733</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>1538825</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>1444225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>2107468</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>1765733</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>1538825</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>1444225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>2107468</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>1765733</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>1538825</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>1444225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>266879</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>246488</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>222070</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>223042</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>2066395</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>1714286</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>1485147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>1388290</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>1723490</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>1412873</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>1210444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>1182431</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>2107468</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>1765733</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>1538825</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>1444225</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>2066395</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>1714286</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>1485147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>1388290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>266879</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>246488</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>222070</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
+        <v>223042</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>25593</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>26176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>26982</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
+        <v>27910</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>25593</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
+        <v>26176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
+        <v>26982</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="3">
+        <v>27910</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361BB3E7-D159-D042-AF80-D3297EB0D283}">
+  <dimension ref="A1:A91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>45382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>1033184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>1033184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>537422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>172353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>596217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>-89331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>-89331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>-81013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>-51009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>-32169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>-417675</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>-417675</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>-309031</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>-367482</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>-129581</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>1502051</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>1502051</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>981795</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>843527</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>1089361</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>234062</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>234062</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>135986</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>192090</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>104068</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>-89365</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>-89365</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>-81025</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>-51017</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>-32218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>9100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>69336</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>-40379</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
+        <v>-69800</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
+        <v>-424905</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>-424905</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
+        <v>-314060</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
+        <v>-370677</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="3">
+        <v>-106579</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="3">
+        <v>943819</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="3">
+        <v>943819</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="3">
+        <v>456397</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="3">
+        <v>121336</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="3">
+        <v>563999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>